<commit_message>
Encoded the banking dataset in "one-hot encoding" in order to do the CNN experiment. Also, wrote the code for the CNN experiment with the banking dataset.
</commit_message>
<xml_diff>
--- a/cnn/results/test_plan.xlsx
+++ b/cnn/results/test_plan.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{20F8A67D-FC00-4EF9-86B0-658CF696CEB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4201B26F-4162-4FA6-9578-7F2A129800B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Figures - Step 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan CIFAR-10" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan Bank" sheetId="3" r:id="rId2"/>
+    <sheet name="Figures - CIFAR Step 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Figures Bank Step 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Step 1 - Learning rate</t>
   </si>
@@ -48,6 +50,27 @@
   </si>
   <si>
     <t>Step 2- Number of epoch</t>
+  </si>
+  <si>
+    <t>Step 1 - Use regular NN as a baseline</t>
+  </si>
+  <si>
+    <t>Baseline with regular NN</t>
+  </si>
+  <si>
+    <t>With Basic CNN LR=0.0001</t>
+  </si>
+  <si>
+    <t>Step 2 - CNN</t>
+  </si>
+  <si>
+    <t>LR=0.0001</t>
+  </si>
+  <si>
+    <t>LR=0.001</t>
+  </si>
+  <si>
+    <t>Learning rate = 0.000001</t>
   </si>
 </sst>
 </file>
@@ -358,6 +381,261 @@
         <a:xfrm>
           <a:off x="7620000" y="14287500"/>
           <a:ext cx="8726118" cy="6716062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>16808</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C1774B-506E-4928-BCCA-A4BD3B3B74E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="6086475"/>
+          <a:ext cx="7598708" cy="5848350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>154770</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78922E1-0462-4F84-B312-D0927C2EA972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="180975"/>
+          <a:ext cx="7391400" cy="5688795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>171731</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A458884B-A933-40EA-80C4-8B7DE2A9FFF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12192000"/>
+          <a:ext cx="7648575" cy="5886731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>153272</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>48403</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 8" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97C1FAAC-718B-49CB-8C80-1B6732064BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="190500"/>
+          <a:ext cx="6249272" cy="5572903"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>153272</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>48403</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B80590-F5C2-4204-BA5E-2DB416505E1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="6096000"/>
+          <a:ext cx="6249272" cy="5572903"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -634,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -712,6 +990,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE9D33-4770-479E-AE0B-821AD2DEF871}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE12AA5-06A4-4772-AF19-176578E02B20}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -724,4 +1037,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656187CF-7292-45C9-A651-C6B5390B2692}">
+  <dimension ref="A1:A96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W40" sqref="W40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Performed a few test runs on the CIFAR-10 dataset. I think all figures / stats required for the "paper" are available for CIFAR-10.
</commit_message>
<xml_diff>
--- a/cnn/results/test_plan.xlsx
+++ b/cnn/results/test_plan.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57ACE4BB-90F8-4AB4-8C0D-C075F720E8D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B4A419A-BD5C-4A8A-AC61-B478EB1A42AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan CIFAR-10" sheetId="1" r:id="rId1"/>
     <sheet name="Plan Bank" sheetId="3" r:id="rId2"/>
     <sheet name="Figures - CIFAR Step 1" sheetId="2" r:id="rId3"/>
     <sheet name="Figures Bank Step 1,2, 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Validation Curve Data" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Step 1 - Learning rate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Using baseline model. 10 epochs</t>
   </si>
@@ -40,18 +38,6 @@
     <t>2018-11-25-16_24_56.txt</t>
   </si>
   <si>
-    <t>Step 2 - Dropout</t>
-  </si>
-  <si>
-    <t>no dropout</t>
-  </si>
-  <si>
-    <t>20 % input dropout</t>
-  </si>
-  <si>
-    <t>Step 2- Number of epoch</t>
-  </si>
-  <si>
     <t>Step 1 - Use regular NN as a baseline</t>
   </si>
   <si>
@@ -77,13 +63,136 @@
   </si>
   <si>
     <t>LR=0.001, Added batch normalization for each layer</t>
+  </si>
+  <si>
+    <t>Second run with Batch Normalization LR=0.001 (2 déc)</t>
+  </si>
+  <si>
+    <t>LR=0.01</t>
+  </si>
+  <si>
+    <t>Batch Norm, LR=0.01</t>
+  </si>
+  <si>
+    <t>Hyper-parameters will be: Learning Rate</t>
+  </si>
+  <si>
+    <t>Training Accuracy</t>
+  </si>
+  <si>
+    <t>Validation Accuracy</t>
+  </si>
+  <si>
+    <t>Using best found learning rate:</t>
+  </si>
+  <si>
+    <t>2018-12-02-15_26_35.txt</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Step 1 - Learning rate @ 10 Epochs</t>
+  </si>
+  <si>
+    <t>Input Dropout Rate (%)</t>
+  </si>
+  <si>
+    <t>Step 2- Input Dropout @ 10 epoch, LR=0.001</t>
+  </si>
+  <si>
+    <t>2018-12-02-15_45_29.txt</t>
+  </si>
+  <si>
+    <t>*Consistent will equivalent run</t>
+  </si>
+  <si>
+    <t>*This one is completely overfitting the data</t>
+  </si>
+  <si>
+    <t>2018-12-02-15_56_30.txt</t>
+  </si>
+  <si>
+    <t>(Trained to 20 epoch, not much improvemtn, still overfit a lot) 79,74% validation accuracy @ 20 epoch with 99% train accuracy.</t>
+  </si>
+  <si>
+    <t>99/78 @ 20 epoch</t>
+  </si>
+  <si>
+    <t>2018-12-02-16_04_41.txt</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>99/77 @ 20 epoch. Still overfitting.</t>
+  </si>
+  <si>
+    <t>Step 3 - Weight Decay, LR=0,001, no dropout</t>
+  </si>
+  <si>
+    <t>Better ratio between training accuracy and validation accuracy.  95/79 @ 20 epoch</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>Improving the ratio, but not the result.</t>
+  </si>
+  <si>
+    <t>2018-12-02-16_28_42.txt</t>
+  </si>
+  <si>
+    <t>2018-12-02-16_36_43.txt</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>2018-12-02-16_49_10.txt</t>
+  </si>
+  <si>
+    <t>2018-12-02-16_54_32.txt</t>
+  </si>
+  <si>
+    <t>Step 4 - Transformations [ Weight Decay=0.001 LR=0.001]</t>
+  </si>
+  <si>
+    <t>Horizontal Flip</t>
+  </si>
+  <si>
+    <t>No Transforms</t>
+  </si>
+  <si>
+    <t>Seems like a huge improvement. The most impact so far.</t>
+  </si>
+  <si>
+    <t>Horizontal Flip + Random Resized Crop 0,85%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gap is close between the two. </t>
+  </si>
+  <si>
+    <t>Horizontal Flip + Random Resized Crop + Random Rotations (10 degrees)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gap is getting even closer. </t>
+  </si>
+  <si>
+    <t>Step 5 - Effect of the number of epoch on the best candidates.</t>
+  </si>
+  <si>
+    <t>(Best candidate is the one with the smallest gap between training accuracy and validation accuracy, since it might benefits from goint to multiple epochs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +202,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,18 +233,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -741,6 +865,106 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="25527000"/>
+          <a:ext cx="8726118" cy="6716062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>344118</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>48562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F67D8A9-2A6C-4300-A6B6-FF4743453FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="32575500"/>
+          <a:ext cx="8726118" cy="6716062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>344118</xdr:colOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>48562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 7" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765B7098-C30E-4BB1-84AE-8D0F71287762}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="39624000"/>
           <a:ext cx="8726118" cy="6716062"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1016,77 +1240,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J30" sqref="B30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <f>B4</f>
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>0.01</v>
       </c>
       <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F7" si="0">B5</f>
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.77129999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.80920000000000003</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="F7">
+        <f t="shared" si="0"/>
         <v>1E-4</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>7</v>
+      <c r="G7" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3">
+        <f>B12</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="3">
+        <f>B13</f>
+        <v>0.05</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3">
+        <f>B14</f>
+        <v>0.1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" t="str">
+        <f>C5</f>
+        <v>2018-11-25-16_19_28.txt</v>
+      </c>
+      <c r="G24" s="3">
+        <f>G6</f>
+        <v>0.98</v>
+      </c>
+      <c r="H24" s="4">
+        <f>H6</f>
+        <v>0.80920000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.82620000000000005</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.79359999999999997</v>
+      </c>
+      <c r="J29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1097,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE9D33-4770-479E-AE0B-821AD2DEF871}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,27 +1632,37 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1142,7 +1674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE12AA5-06A4-4772-AF19-176578E02B20}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -1155,41 +1687,69 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656187CF-7292-45C9-A651-C6B5390B2692}">
-  <dimension ref="A1:A134"/>
+  <dimension ref="A1:A208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O219" sqref="O218:O219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1777BA90-2DD7-4AAF-BA19-6AC5D7CAD1B7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prepared figures for the banking dataset. Added confusion matrix for 10000 samples.
</commit_message>
<xml_diff>
--- a/cnn/results/test_plan.xlsx
+++ b/cnn/results/test_plan.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B4A419A-BD5C-4A8A-AC61-B478EB1A42AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D14D2E1F-A593-43B7-842A-3017B680A13E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan CIFAR-10" sheetId="1" r:id="rId1"/>
     <sheet name="Plan Bank" sheetId="3" r:id="rId2"/>
     <sheet name="Figures - CIFAR Step 1" sheetId="2" r:id="rId3"/>
-    <sheet name="Figures Bank Step 1,2, 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Validation Curve Data" sheetId="5" r:id="rId5"/>
+    <sheet name="Figures - Banking" sheetId="6" r:id="rId4"/>
+    <sheet name="Old - Figures Bank Step 1,2, 3" sheetId="4" r:id="rId5"/>
+    <sheet name="Validation Curve Data" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="104">
   <si>
     <t>Using baseline model. 10 epochs</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Learning rate = 0.000001</t>
   </si>
   <si>
-    <t>Step 3 - CNN With Batch Normalization on all layers</t>
-  </si>
-  <si>
     <t>LR=0.001, Added batch normalization for each layer</t>
   </si>
   <si>
@@ -186,6 +184,159 @@
   </si>
   <si>
     <t>(Best candidate is the one with the smallest gap between training accuracy and validation accuracy, since it might benefits from goint to multiple epochs</t>
+  </si>
+  <si>
+    <t>LR=0.1</t>
+  </si>
+  <si>
+    <t>CNN with batch normalization.</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>2018-12-08-10_36_49.txt</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>90.42</t>
+  </si>
+  <si>
+    <t>2018-12-08-10_44_05.txt</t>
+  </si>
+  <si>
+    <t>90.54</t>
+  </si>
+  <si>
+    <t>Test F1</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>2018-12-08-10_49_53.txt</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>90.11</t>
+  </si>
+  <si>
+    <t>Test "Yes" F1</t>
+  </si>
+  <si>
+    <t>89.76</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>2018-12-08-10_55_54.txt</t>
+  </si>
+  <si>
+    <t>LR=1</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>89.91</t>
+  </si>
+  <si>
+    <t>(Recall)</t>
+  </si>
+  <si>
+    <t>Test Precision</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>2018-12-08-11_04_30.txt</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>Batch Size</t>
+  </si>
+  <si>
+    <t>Step 3 - Batch Size -  Using best "Test Yes F1 score" LR = 0.0001</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>90.47</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>2018-12-08-11_24_11.txt</t>
+  </si>
+  <si>
+    <t>*Overall best result!</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>0.9136</t>
+  </si>
+  <si>
+    <t>2018-12-08-12_52_10.txt</t>
+  </si>
+  <si>
+    <t>Batch Size = 10, maybe some luck</t>
+  </si>
+  <si>
+    <t>2018-12-08-13_07_28.txt</t>
+  </si>
+  <si>
+    <t>90.19</t>
+  </si>
+  <si>
+    <t>2018-12-08-13_16_10.txt</t>
+  </si>
+  <si>
+    <t>2018-12-08-14_51_05.txt</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>86.319</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.00001</t>
+  </si>
+  <si>
+    <t>0.000001</t>
   </si>
 </sst>
 </file>
@@ -237,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -249,6 +400,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,6 +675,111 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>344118</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>48562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE5A8A70-B497-494A-84B4-0A5016F936E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="8726118" cy="6716062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>344118</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>48562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4" descr="Figure 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B17C421-6BD2-4670-8EBD-2C598CCDB05D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7239000"/>
+          <a:ext cx="8726118" cy="6716062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1242,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J30" sqref="B30:J30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,16 +1518,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,7 +1535,7 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <f>B4</f>
@@ -1327,7 +1584,7 @@
         <v>0.80920000000000003</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1350,21 +1607,21 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3">
         <f>B12</f>
@@ -1385,7 +1642,7 @@
         <v>0.80700000000000005</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1393,7 +1650,7 @@
         <v>0.05</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3">
         <f>B13</f>
@@ -1406,7 +1663,7 @@
         <v>0.79</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1414,7 +1671,7 @@
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3">
         <f>B14</f>
@@ -1427,7 +1684,7 @@
         <v>0.79</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1435,7 +1692,7 @@
         <v>0.15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3">
         <v>0.15</v>
@@ -1447,7 +1704,7 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1461,15 +1718,15 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" s="3">
         <v>0.62</v>
@@ -1480,10 +1737,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="3">
         <v>0.78</v>
@@ -1494,10 +1751,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="3">
         <v>0.89</v>
@@ -1506,15 +1763,15 @@
         <v>0.8</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="3">
         <v>0.95</v>
@@ -1523,7 +1780,7 @@
         <v>0.8</v>
       </c>
       <c r="J23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1545,12 +1802,12 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G27" s="3">
         <v>0.89</v>
@@ -1561,7 +1818,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="3">
         <v>0.85</v>
@@ -1570,12 +1827,12 @@
         <v>0.82620000000000005</v>
       </c>
       <c r="J28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G29" s="3">
         <v>0.81</v>
@@ -1584,12 +1841,12 @@
         <v>0.79359999999999997</v>
       </c>
       <c r="J29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G30" s="3">
         <v>0.79</v>
@@ -1598,17 +1855,17 @@
         <v>0.78</v>
       </c>
       <c r="J30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1619,54 +1876,433 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE9D33-4770-479E-AE0B-821AD2DEF871}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20">
+        <v>1000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1674,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE12AA5-06A4-4772-AF19-176578E02B20}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -1686,10 +2322,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8BEC77-A4C1-45CA-B71A-A8039B30FDF5}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656187CF-7292-45C9-A651-C6B5390B2692}">
   <dimension ref="A1:A208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A223" workbookViewId="0">
       <selection activeCell="O219" sqref="O218:O219"/>
     </sheetView>
   </sheetViews>
@@ -1717,17 +2379,17 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1736,7 +2398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1777BA90-2DD7-4AAF-BA19-6AC5D7CAD1B7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1746,7 +2408,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>